<commit_message>
The three versions of the HWP model (base, Sankey, MC) all include PIU loss values for paper (pulp) and wood separately.  Template and existing input files allow users to alter these values.  This mainly affects the display of the Sankey diagram.  .Rmd files updated.
</commit_message>
<xml_diff>
--- a/HWP Data/ExistingData/CA_DiscardEnergyCapture_Test.xlsx
+++ b/HWP Data/ExistingData/CA_DiscardEnergyCapture_Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\RSTUDIO_GIT_PROJECTS\HWP_Shared_Test\HWP Data\ExistingData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\RSTUDIO_GIT_PROJECTS\HWP-C-vR\HWP Data\ExistingData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60DD708-33D3-40BC-BADB-7A8552B768FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56020C7E-FAD6-44E4-86C5-BAD56B7D2156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29190" yWindow="540" windowWidth="21600" windowHeight="20520" tabRatio="767" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29565" yWindow="1350" windowWidth="28800" windowHeight="15435" tabRatio="767" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HWP_MODEL_OPTIONS" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="126">
   <si>
     <t>QA_TEST</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>SHIFTYEAR</t>
-  </si>
-  <si>
-    <t>PIU.LOSS</t>
   </si>
   <si>
     <t>ARRAYLOC</t>
@@ -417,6 +414,12 @@
   </si>
   <si>
     <t>DEC</t>
+  </si>
+  <si>
+    <t>PIU.WOOD.LOSS</t>
+  </si>
+  <si>
+    <t>PIU.PAPER.LOSS</t>
   </si>
 </sst>
 </file>
@@ -1264,17 +1267,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+      <selection activeCell="F1" sqref="F1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1289,33 +1292,36 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -1332,25 +1338,28 @@
       <c r="F2">
         <v>0.08</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>121</v>
+      </c>
+      <c r="I2" t="s">
         <v>122</v>
       </c>
-      <c r="H2" t="s">
-        <v>123</v>
-      </c>
-      <c r="I2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0.5</v>
+      <c r="J2" t="b">
+        <v>0</v>
       </c>
       <c r="K2">
         <v>0.5</v>
       </c>
       <c r="L2">
+        <v>0.5</v>
+      </c>
+      <c r="M2">
         <v>100</v>
       </c>
-      <c r="M2" t="b">
+      <c r="N2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1371,10 +1380,10 @@
   <sheetData>
     <row r="1" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" t="s">
         <v>88</v>
-      </c>
-      <c r="B1" t="s">
-        <v>89</v>
       </c>
       <c r="C1">
         <v>1952</v>
@@ -1583,10 +1592,10 @@
     </row>
     <row r="2" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1795,10 +1804,10 @@
     </row>
     <row r="3" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2007,10 +2016,10 @@
     </row>
     <row r="4" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C4">
         <v>0.3</v>
@@ -2219,10 +2228,10 @@
     </row>
     <row r="5" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" t="s">
         <v>91</v>
-      </c>
-      <c r="B5" t="s">
-        <v>92</v>
       </c>
       <c r="C5">
         <v>0.3</v>
@@ -2431,10 +2440,10 @@
     </row>
     <row r="6" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -2643,10 +2652,10 @@
     </row>
     <row r="7" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -2855,10 +2864,10 @@
     </row>
     <row r="8" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -3067,10 +3076,10 @@
     </row>
     <row r="9" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -3279,10 +3288,10 @@
     </row>
     <row r="10" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C10">
         <v>7.0000000000000007E-2</v>
@@ -3491,10 +3500,10 @@
     </row>
     <row r="11" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C11">
         <v>7.0000000000000007E-2</v>
@@ -3703,10 +3712,10 @@
     </row>
     <row r="12" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C12">
         <v>0.63</v>
@@ -3915,10 +3924,10 @@
     </row>
     <row r="13" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C13">
         <v>0.63</v>
@@ -4147,24 +4156,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" t="s">
         <v>97</v>
       </c>
-      <c r="B1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>98</v>
       </c>
-      <c r="D1" t="s">
-        <v>99</v>
-      </c>
       <c r="E1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2">
         <v>8.25</v>
@@ -4181,7 +4190,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3">
         <v>16.5</v>
@@ -4213,31 +4222,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
         <v>100</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>101</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>102</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>103</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>104</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>105</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>106</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>107</v>
-      </c>
-      <c r="I1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -4245,7 +4254,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F2">
         <v>0.95</v>
@@ -4265,7 +4274,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F3">
         <v>0.85</v>
@@ -4285,7 +4294,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F4">
         <v>0.85</v>
@@ -4305,7 +4314,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -4328,7 +4337,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -4351,7 +4360,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -4374,7 +4383,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -4397,7 +4406,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -4420,7 +4429,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -4443,7 +4452,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -4466,7 +4475,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -4489,7 +4498,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -4512,7 +4521,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -4535,7 +4544,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D15">
         <v>1952</v>
@@ -4561,7 +4570,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D16">
         <v>1980</v>
@@ -4587,7 +4596,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D17">
         <v>1952</v>
@@ -4613,7 +4622,7 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D18">
         <v>1980</v>
@@ -4639,7 +4648,7 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D19">
         <v>1952</v>
@@ -4665,7 +4674,7 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D20">
         <v>1980</v>
@@ -4703,25 +4712,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
         <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -6310,13 +6319,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -6402,7 +6411,7 @@
   <sheetData>
     <row r="1" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1">
         <v>1952</v>
@@ -14986,7 +14995,7 @@
   <sheetData>
     <row r="1" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1">
         <v>1952</v>
@@ -28586,7 +28595,7 @@
   <sheetData>
     <row r="1" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1">
         <v>1952</v>
@@ -75626,22 +75635,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>26</v>
-      </c>
-      <c r="F1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -75655,13 +75664,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -75675,13 +75684,13 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
         <v>30</v>
-      </c>
-      <c r="F3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -75695,13 +75704,13 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -75715,13 +75724,13 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -75735,13 +75744,13 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -75755,13 +75764,13 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -75775,13 +75784,13 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -75795,13 +75804,13 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -75815,13 +75824,13 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -75835,13 +75844,13 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -75855,13 +75864,13 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -75875,13 +75884,13 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -75895,13 +75904,13 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -75915,13 +75924,13 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -75935,13 +75944,13 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -75955,13 +75964,13 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -75975,13 +75984,13 @@
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -75995,13 +76004,13 @@
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -76015,13 +76024,13 @@
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -76035,13 +76044,13 @@
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -76055,13 +76064,13 @@
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -76075,13 +76084,13 @@
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -76095,13 +76104,13 @@
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -76115,13 +76124,13 @@
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -76135,13 +76144,13 @@
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -76155,13 +76164,13 @@
         <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -76175,13 +76184,13 @@
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -76195,13 +76204,13 @@
         <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -76215,13 +76224,13 @@
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -76235,13 +76244,13 @@
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -76255,13 +76264,13 @@
         <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -76275,13 +76284,13 @@
         <v>32</v>
       </c>
       <c r="D33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -76295,13 +76304,13 @@
         <v>33</v>
       </c>
       <c r="D34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -76315,13 +76324,13 @@
         <v>34</v>
       </c>
       <c r="D35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -76335,13 +76344,13 @@
         <v>35</v>
       </c>
       <c r="D36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -76355,13 +76364,13 @@
         <v>36</v>
       </c>
       <c r="D37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -76375,13 +76384,13 @@
         <v>37</v>
       </c>
       <c r="D38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -76395,13 +76404,13 @@
         <v>38</v>
       </c>
       <c r="D39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -76415,13 +76424,13 @@
         <v>39</v>
       </c>
       <c r="D40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -76435,13 +76444,13 @@
         <v>40</v>
       </c>
       <c r="D41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -76455,13 +76464,13 @@
         <v>41</v>
       </c>
       <c r="D42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -76475,13 +76484,13 @@
         <v>42</v>
       </c>
       <c r="D43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -76495,13 +76504,13 @@
         <v>43</v>
       </c>
       <c r="D44" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -76515,13 +76524,13 @@
         <v>44</v>
       </c>
       <c r="D45" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F45" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -76535,13 +76544,13 @@
         <v>45</v>
       </c>
       <c r="D46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -76555,13 +76564,13 @@
         <v>46</v>
       </c>
       <c r="D47" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F47" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -76575,13 +76584,13 @@
         <v>47</v>
       </c>
       <c r="D48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -76595,13 +76604,13 @@
         <v>48</v>
       </c>
       <c r="D49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -76615,13 +76624,13 @@
         <v>49</v>
       </c>
       <c r="D50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F50" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -76635,13 +76644,13 @@
         <v>50</v>
       </c>
       <c r="D51" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E51" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F51" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -76655,13 +76664,13 @@
         <v>51</v>
       </c>
       <c r="D52" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E52" t="s">
+        <v>29</v>
+      </c>
+      <c r="F52" t="s">
         <v>30</v>
-      </c>
-      <c r="F52" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -76675,13 +76684,13 @@
         <v>52</v>
       </c>
       <c r="D53" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E53" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F53" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -76695,13 +76704,13 @@
         <v>53</v>
       </c>
       <c r="D54" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E54" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F54" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -76715,13 +76724,13 @@
         <v>54</v>
       </c>
       <c r="D55" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E55" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F55" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -76735,13 +76744,13 @@
         <v>55</v>
       </c>
       <c r="D56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E56" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F56" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -76755,13 +76764,13 @@
         <v>56</v>
       </c>
       <c r="D57" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E57" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -76775,13 +76784,13 @@
         <v>57</v>
       </c>
       <c r="D58" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E58" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F58" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -76795,13 +76804,13 @@
         <v>58</v>
       </c>
       <c r="D59" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E59" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F59" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -76815,13 +76824,13 @@
         <v>59</v>
       </c>
       <c r="D60" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E60" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F60" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -76835,13 +76844,13 @@
         <v>60</v>
       </c>
       <c r="D61" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E61" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F61" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -76855,13 +76864,13 @@
         <v>61</v>
       </c>
       <c r="D62" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E62" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F62" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -76875,13 +76884,13 @@
         <v>62</v>
       </c>
       <c r="D63" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E63" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F63" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -76895,13 +76904,13 @@
         <v>63</v>
       </c>
       <c r="D64" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E64" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F64" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -76915,13 +76924,13 @@
         <v>64</v>
       </c>
       <c r="D65" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E65" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F65" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -76935,13 +76944,13 @@
         <v>65</v>
       </c>
       <c r="D66" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E66" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F66" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -76955,13 +76964,13 @@
         <v>66</v>
       </c>
       <c r="D67" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E67" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F67" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -76975,13 +76984,13 @@
         <v>67</v>
       </c>
       <c r="D68" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E68" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F68" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -76995,13 +77004,13 @@
         <v>68</v>
       </c>
       <c r="D69" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E69" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F69" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -77015,13 +77024,13 @@
         <v>69</v>
       </c>
       <c r="D70" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E70" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F70" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -77035,13 +77044,13 @@
         <v>70</v>
       </c>
       <c r="D71" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E71" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F71" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -77055,13 +77064,13 @@
         <v>71</v>
       </c>
       <c r="D72" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E72" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F72" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -77075,13 +77084,13 @@
         <v>72</v>
       </c>
       <c r="D73" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E73" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F73" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -77095,13 +77104,13 @@
         <v>73</v>
       </c>
       <c r="D74" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E74" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F74" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -77115,13 +77124,13 @@
         <v>74</v>
       </c>
       <c r="D75" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E75" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F75" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -77135,13 +77144,13 @@
         <v>75</v>
       </c>
       <c r="D76" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E76" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F76" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -77155,13 +77164,13 @@
         <v>76</v>
       </c>
       <c r="D77" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E77" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F77" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -77175,13 +77184,13 @@
         <v>77</v>
       </c>
       <c r="D78" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E78" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F78" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -77195,13 +77204,13 @@
         <v>78</v>
       </c>
       <c r="D79" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E79" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F79" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -77215,13 +77224,13 @@
         <v>79</v>
       </c>
       <c r="D80" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E80" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F80" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -77235,13 +77244,13 @@
         <v>80</v>
       </c>
       <c r="D81" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E81" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F81" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -77255,13 +77264,13 @@
         <v>81</v>
       </c>
       <c r="D82" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E82" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F82" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -77275,13 +77284,13 @@
         <v>82</v>
       </c>
       <c r="D83" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E83" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F83" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -77295,13 +77304,13 @@
         <v>83</v>
       </c>
       <c r="D84" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E84" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F84" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -77315,13 +77324,13 @@
         <v>84</v>
       </c>
       <c r="D85" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E85" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F85" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -77335,13 +77344,13 @@
         <v>85</v>
       </c>
       <c r="D86" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E86" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F86" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -77355,13 +77364,13 @@
         <v>86</v>
       </c>
       <c r="D87" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E87" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F87" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -77375,13 +77384,13 @@
         <v>87</v>
       </c>
       <c r="D88" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E88" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F88" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -77395,13 +77404,13 @@
         <v>88</v>
       </c>
       <c r="D89" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E89" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F89" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -77415,13 +77424,13 @@
         <v>89</v>
       </c>
       <c r="D90" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E90" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F90" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -77435,13 +77444,13 @@
         <v>90</v>
       </c>
       <c r="D91" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E91" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F91" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -77455,13 +77464,13 @@
         <v>91</v>
       </c>
       <c r="D92" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E92" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F92" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -77475,13 +77484,13 @@
         <v>92</v>
       </c>
       <c r="D93" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E93" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F93" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -77495,13 +77504,13 @@
         <v>93</v>
       </c>
       <c r="D94" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E94" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F94" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -77515,13 +77524,13 @@
         <v>94</v>
       </c>
       <c r="D95" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E95" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F95" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -77535,13 +77544,13 @@
         <v>95</v>
       </c>
       <c r="D96" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E96" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F96" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -77555,13 +77564,13 @@
         <v>96</v>
       </c>
       <c r="D97" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E97" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F97" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -77575,13 +77584,13 @@
         <v>97</v>
       </c>
       <c r="D98" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E98" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F98" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -77595,13 +77604,13 @@
         <v>98</v>
       </c>
       <c r="D99" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E99" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F99" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -77615,13 +77624,13 @@
         <v>99</v>
       </c>
       <c r="D100" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E100" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F100" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -77635,13 +77644,13 @@
         <v>100</v>
       </c>
       <c r="D101" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E101" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F101" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -77655,13 +77664,13 @@
         <v>101</v>
       </c>
       <c r="D102" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E102" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F102" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -77675,13 +77684,13 @@
         <v>102</v>
       </c>
       <c r="D103" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E103" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F103" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -77695,13 +77704,13 @@
         <v>103</v>
       </c>
       <c r="D104" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E104" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F104" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -77715,13 +77724,13 @@
         <v>104</v>
       </c>
       <c r="D105" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E105" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F105" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -77735,13 +77744,13 @@
         <v>105</v>
       </c>
       <c r="D106" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E106" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F106" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -77755,13 +77764,13 @@
         <v>106</v>
       </c>
       <c r="D107" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E107" t="s">
+        <v>29</v>
+      </c>
+      <c r="F107" t="s">
         <v>30</v>
-      </c>
-      <c r="F107" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -77775,13 +77784,13 @@
         <v>107</v>
       </c>
       <c r="D108" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E108" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F108" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -77795,13 +77804,13 @@
         <v>108</v>
       </c>
       <c r="D109" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E109" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F109" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -77815,13 +77824,13 @@
         <v>109</v>
       </c>
       <c r="D110" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E110" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F110" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -77835,13 +77844,13 @@
         <v>110</v>
       </c>
       <c r="D111" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E111" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F111" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -77855,13 +77864,13 @@
         <v>111</v>
       </c>
       <c r="D112" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E112" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F112" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -77875,13 +77884,13 @@
         <v>112</v>
       </c>
       <c r="D113" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E113" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F113" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -77895,13 +77904,13 @@
         <v>113</v>
       </c>
       <c r="D114" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E114" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F114" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -77915,13 +77924,13 @@
         <v>114</v>
       </c>
       <c r="D115" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E115" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F115" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -77935,13 +77944,13 @@
         <v>115</v>
       </c>
       <c r="D116" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E116" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F116" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -77955,13 +77964,13 @@
         <v>116</v>
       </c>
       <c r="D117" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E117" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F117" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -77975,13 +77984,13 @@
         <v>117</v>
       </c>
       <c r="D118" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E118" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F118" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -77995,13 +78004,13 @@
         <v>118</v>
       </c>
       <c r="D119" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E119" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F119" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -78015,13 +78024,13 @@
         <v>119</v>
       </c>
       <c r="D120" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E120" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F120" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -78035,13 +78044,13 @@
         <v>120</v>
       </c>
       <c r="D121" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E121" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F121" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -78055,13 +78064,13 @@
         <v>121</v>
       </c>
       <c r="D122" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E122" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F122" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -78075,13 +78084,13 @@
         <v>122</v>
       </c>
       <c r="D123" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E123" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F123" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -78095,13 +78104,13 @@
         <v>123</v>
       </c>
       <c r="D124" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E124" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F124" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -78115,13 +78124,13 @@
         <v>124</v>
       </c>
       <c r="D125" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E125" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F125" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -78135,13 +78144,13 @@
         <v>125</v>
       </c>
       <c r="D126" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E126" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F126" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -78155,13 +78164,13 @@
         <v>126</v>
       </c>
       <c r="D127" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E127" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F127" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -78175,13 +78184,13 @@
         <v>127</v>
       </c>
       <c r="D128" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E128" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F128" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -78195,13 +78204,13 @@
         <v>128</v>
       </c>
       <c r="D129" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E129" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F129" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
@@ -78215,13 +78224,13 @@
         <v>129</v>
       </c>
       <c r="D130" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E130" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F130" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
@@ -78235,13 +78244,13 @@
         <v>130</v>
       </c>
       <c r="D131" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E131" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F131" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
@@ -78255,13 +78264,13 @@
         <v>131</v>
       </c>
       <c r="D132" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E132" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
@@ -78275,13 +78284,13 @@
         <v>132</v>
       </c>
       <c r="D133" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E133" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F133" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
@@ -78295,13 +78304,13 @@
         <v>133</v>
       </c>
       <c r="D134" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E134" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F134" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
@@ -78315,13 +78324,13 @@
         <v>134</v>
       </c>
       <c r="D135" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E135" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F135" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
@@ -78335,13 +78344,13 @@
         <v>135</v>
       </c>
       <c r="D136" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E136" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F136" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
@@ -78355,13 +78364,13 @@
         <v>136</v>
       </c>
       <c r="D137" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E137" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F137" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
@@ -78375,13 +78384,13 @@
         <v>137</v>
       </c>
       <c r="D138" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E138" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F138" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
@@ -78395,13 +78404,13 @@
         <v>138</v>
       </c>
       <c r="D139" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E139" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F139" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
@@ -78415,13 +78424,13 @@
         <v>139</v>
       </c>
       <c r="D140" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E140" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F140" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
@@ -78435,13 +78444,13 @@
         <v>140</v>
       </c>
       <c r="D141" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E141" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F141" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
@@ -78455,13 +78464,13 @@
         <v>141</v>
       </c>
       <c r="D142" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E142" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F142" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
@@ -78475,13 +78484,13 @@
         <v>142</v>
       </c>
       <c r="D143" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E143" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F143" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
@@ -78495,13 +78504,13 @@
         <v>143</v>
       </c>
       <c r="D144" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E144" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F144" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
@@ -78515,13 +78524,13 @@
         <v>144</v>
       </c>
       <c r="D145" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E145" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F145" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
@@ -78535,13 +78544,13 @@
         <v>145</v>
       </c>
       <c r="D146" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E146" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F146" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
@@ -78555,13 +78564,13 @@
         <v>146</v>
       </c>
       <c r="D147" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E147" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F147" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
@@ -78575,13 +78584,13 @@
         <v>147</v>
       </c>
       <c r="D148" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E148" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F148" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
@@ -78595,13 +78604,13 @@
         <v>148</v>
       </c>
       <c r="D149" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E149" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F149" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
@@ -78615,13 +78624,13 @@
         <v>149</v>
       </c>
       <c r="D150" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E150" t="s">
+        <v>29</v>
+      </c>
+      <c r="F150" t="s">
         <v>30</v>
-      </c>
-      <c r="F150" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -78635,13 +78644,13 @@
         <v>150</v>
       </c>
       <c r="D151" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E151" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F151" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
@@ -78655,13 +78664,13 @@
         <v>151</v>
       </c>
       <c r="D152" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E152" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F152" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
@@ -78675,13 +78684,13 @@
         <v>152</v>
       </c>
       <c r="D153" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E153" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F153" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -78695,13 +78704,13 @@
         <v>153</v>
       </c>
       <c r="D154" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E154" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F154" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -78715,13 +78724,13 @@
         <v>154</v>
       </c>
       <c r="D155" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E155" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F155" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -78735,13 +78744,13 @@
         <v>155</v>
       </c>
       <c r="D156" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E156" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F156" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -78755,13 +78764,13 @@
         <v>156</v>
       </c>
       <c r="D157" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E157" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F157" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -78775,13 +78784,13 @@
         <v>157</v>
       </c>
       <c r="D158" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E158" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F158" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -78795,13 +78804,13 @@
         <v>158</v>
       </c>
       <c r="D159" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E159" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F159" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -78815,13 +78824,13 @@
         <v>159</v>
       </c>
       <c r="D160" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E160" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F160" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -78835,13 +78844,13 @@
         <v>160</v>
       </c>
       <c r="D161" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E161" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F161" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
@@ -78855,13 +78864,13 @@
         <v>161</v>
       </c>
       <c r="D162" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E162" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F162" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -78875,13 +78884,13 @@
         <v>162</v>
       </c>
       <c r="D163" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E163" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F163" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -78895,13 +78904,13 @@
         <v>163</v>
       </c>
       <c r="D164" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E164" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F164" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -78915,13 +78924,13 @@
         <v>164</v>
       </c>
       <c r="D165" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E165" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F165" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -78935,13 +78944,13 @@
         <v>165</v>
       </c>
       <c r="D166" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E166" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F166" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -78955,13 +78964,13 @@
         <v>166</v>
       </c>
       <c r="D167" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E167" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F167" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
@@ -78975,13 +78984,13 @@
         <v>167</v>
       </c>
       <c r="D168" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E168" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F168" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
@@ -78995,13 +79004,13 @@
         <v>168</v>
       </c>
       <c r="D169" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E169" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F169" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
@@ -79015,13 +79024,13 @@
         <v>169</v>
       </c>
       <c r="D170" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E170" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F170" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
@@ -79035,13 +79044,13 @@
         <v>170</v>
       </c>
       <c r="D171" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E171" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F171" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
@@ -79055,13 +79064,13 @@
         <v>171</v>
       </c>
       <c r="D172" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E172" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F172" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -79075,13 +79084,13 @@
         <v>172</v>
       </c>
       <c r="D173" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E173" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F173" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -79095,13 +79104,13 @@
         <v>173</v>
       </c>
       <c r="D174" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E174" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F174" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
@@ -79115,13 +79124,13 @@
         <v>174</v>
       </c>
       <c r="D175" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E175" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F175" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
@@ -79135,13 +79144,13 @@
         <v>175</v>
       </c>
       <c r="D176" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E176" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F176" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
@@ -79155,13 +79164,13 @@
         <v>176</v>
       </c>
       <c r="D177" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E177" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F177" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
@@ -79175,13 +79184,13 @@
         <v>177</v>
       </c>
       <c r="D178" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E178" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F178" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
@@ -79195,13 +79204,13 @@
         <v>178</v>
       </c>
       <c r="D179" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E179" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F179" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
@@ -79215,13 +79224,13 @@
         <v>179</v>
       </c>
       <c r="D180" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E180" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F180" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
@@ -79235,13 +79244,13 @@
         <v>180</v>
       </c>
       <c r="D181" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E181" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F181" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
@@ -79255,13 +79264,13 @@
         <v>181</v>
       </c>
       <c r="D182" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E182" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F182" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
@@ -79275,13 +79284,13 @@
         <v>182</v>
       </c>
       <c r="D183" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E183" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F183" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
@@ -79295,13 +79304,13 @@
         <v>183</v>
       </c>
       <c r="D184" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E184" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F184" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
@@ -79315,13 +79324,13 @@
         <v>184</v>
       </c>
       <c r="D185" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E185" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F185" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
@@ -79335,13 +79344,13 @@
         <v>185</v>
       </c>
       <c r="D186" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E186" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F186" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
@@ -79355,13 +79364,13 @@
         <v>186</v>
       </c>
       <c r="D187" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E187" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F187" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
@@ -79375,13 +79384,13 @@
         <v>187</v>
       </c>
       <c r="D188" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E188" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F188" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
@@ -79395,13 +79404,13 @@
         <v>188</v>
       </c>
       <c r="D189" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E189" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F189" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
@@ -79415,13 +79424,13 @@
         <v>189</v>
       </c>
       <c r="D190" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E190" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F190" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
@@ -79435,13 +79444,13 @@
         <v>190</v>
       </c>
       <c r="D191" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E191" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F191" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
@@ -79455,13 +79464,13 @@
         <v>191</v>
       </c>
       <c r="D192" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E192" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F192" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
@@ -79475,13 +79484,13 @@
         <v>192</v>
       </c>
       <c r="D193" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E193" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F193" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
@@ -79495,13 +79504,13 @@
         <v>193</v>
       </c>
       <c r="D194" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E194" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F194" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
@@ -79515,13 +79524,13 @@
         <v>194</v>
       </c>
       <c r="D195" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E195" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F195" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
@@ -79535,13 +79544,13 @@
         <v>195</v>
       </c>
       <c r="D196" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E196" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F196" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
@@ -79555,13 +79564,13 @@
         <v>196</v>
       </c>
       <c r="D197" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E197" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F197" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
@@ -79575,13 +79584,13 @@
         <v>197</v>
       </c>
       <c r="D198" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E198" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F198" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
@@ -79595,13 +79604,13 @@
         <v>198</v>
       </c>
       <c r="D199" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E199" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F199" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
@@ -79615,13 +79624,13 @@
         <v>199</v>
       </c>
       <c r="D200" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E200" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F200" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
@@ -79635,13 +79644,13 @@
         <v>200</v>
       </c>
       <c r="D201" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E201" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F201" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
@@ -79655,13 +79664,13 @@
         <v>201</v>
       </c>
       <c r="D202" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E202" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F202" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
@@ -79675,13 +79684,13 @@
         <v>202</v>
       </c>
       <c r="D203" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E203" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F203" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
@@ -79695,13 +79704,13 @@
         <v>203</v>
       </c>
       <c r="D204" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E204" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F204" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
@@ -79715,13 +79724,13 @@
         <v>204</v>
       </c>
       <c r="D205" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E205" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F205" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
@@ -79735,13 +79744,13 @@
         <v>205</v>
       </c>
       <c r="D206" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E206" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F206" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
@@ -79755,13 +79764,13 @@
         <v>206</v>
       </c>
       <c r="D207" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E207" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F207" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
@@ -79775,13 +79784,13 @@
         <v>207</v>
       </c>
       <c r="D208" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E208" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F208" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
@@ -79795,13 +79804,13 @@
         <v>208</v>
       </c>
       <c r="D209" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E209" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F209" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
@@ -79815,13 +79824,13 @@
         <v>209</v>
       </c>
       <c r="D210" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E210" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F210" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
@@ -79835,13 +79844,13 @@
         <v>210</v>
       </c>
       <c r="D211" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E211" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F211" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
@@ -79855,13 +79864,13 @@
         <v>211</v>
       </c>
       <c r="D212" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E212" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F212" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
@@ -79875,13 +79884,13 @@
         <v>212</v>
       </c>
       <c r="D213" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E213" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F213" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
@@ -79895,13 +79904,13 @@
         <v>213</v>
       </c>
       <c r="D214" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E214" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F214" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
@@ -79915,13 +79924,13 @@
         <v>214</v>
       </c>
       <c r="D215" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E215" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F215" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
@@ -79935,13 +79944,13 @@
         <v>215</v>
       </c>
       <c r="D216" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E216" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F216" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
@@ -79955,13 +79964,13 @@
         <v>216</v>
       </c>
       <c r="D217" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E217" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F217" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
@@ -79975,13 +79984,13 @@
         <v>217</v>
       </c>
       <c r="D218" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E218" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F218" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
@@ -79995,13 +80004,13 @@
         <v>218</v>
       </c>
       <c r="D219" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E219" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F219" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
@@ -80015,13 +80024,13 @@
         <v>219</v>
       </c>
       <c r="D220" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E220" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F220" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
@@ -80035,13 +80044,13 @@
         <v>220</v>
       </c>
       <c r="D221" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E221" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F221" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
@@ -80055,13 +80064,13 @@
         <v>221</v>
       </c>
       <c r="D222" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E222" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F222" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
@@ -80075,13 +80084,13 @@
         <v>222</v>
       </c>
       <c r="D223" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E223" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F223" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
@@ -80095,13 +80104,13 @@
         <v>223</v>
       </c>
       <c r="D224" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E224" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F224" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
@@ -80115,13 +80124,13 @@
         <v>224</v>
       </c>
       <c r="D225" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E225" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F225" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -80141,10 +80150,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -80676,10 +80685,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated all references from board feet and cubic feet (e.g., Harvest_BF, bfcf.hwp) to thousand board feet / hundred cubic feet (Harvest_MBF, mbfccf.hwp).
</commit_message>
<xml_diff>
--- a/HWP Data/ExistingData/CA_DiscardEnergyCapture_Test.xlsx
+++ b/HWP Data/ExistingData/CA_DiscardEnergyCapture_Test.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\RSTUDIO_GIT_PROJECTS\HWP-C-vR\HWP Data\ExistingData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56020C7E-FAD6-44E4-86C5-BAD56B7D2156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9166293B-2FFA-43D7-BCD6-EDF667CA993F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29565" yWindow="1350" windowWidth="28800" windowHeight="15435" tabRatio="767" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="767" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HWP_MODEL_OPTIONS" sheetId="1" r:id="rId1"/>
-    <sheet name="Harvest_BF" sheetId="3" r:id="rId2"/>
-    <sheet name="BFCF" sheetId="4" r:id="rId3"/>
+    <sheet name="Harvest_MBF" sheetId="3" r:id="rId2"/>
+    <sheet name="MBFCCF" sheetId="4" r:id="rId3"/>
     <sheet name="TimberProdRatios" sheetId="5" r:id="rId4"/>
     <sheet name="PrimaryProdRatios" sheetId="6" r:id="rId5"/>
     <sheet name="EndUseRatios" sheetId="7" r:id="rId6"/>
@@ -1269,7 +1269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1:G2"/>
     </sheetView>
   </sheetViews>
@@ -6306,8 +6306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Transitioned back from MBFCCF references and template worksheet names to BFCF: all code again references BFCF or versions of bfcf*.  Data files corrected as well.
</commit_message>
<xml_diff>
--- a/HWP Data/ExistingData/CA_DiscardEnergyCapture_Test.xlsx
+++ b/HWP Data/ExistingData/CA_DiscardEnergyCapture_Test.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\RSTUDIO_GIT_PROJECTS\HWP-C-vR\HWP Data\ExistingData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9166293B-2FFA-43D7-BCD6-EDF667CA993F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E83A45C-2D6A-4D41-802D-59E179DB22CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="767" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33495" yWindow="1005" windowWidth="24870" windowHeight="15600" tabRatio="767" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HWP_MODEL_OPTIONS" sheetId="1" r:id="rId1"/>
     <sheet name="Harvest_MBF" sheetId="3" r:id="rId2"/>
-    <sheet name="MBFCCF" sheetId="4" r:id="rId3"/>
+    <sheet name="BFCF" sheetId="4" r:id="rId3"/>
     <sheet name="TimberProdRatios" sheetId="5" r:id="rId4"/>
     <sheet name="PrimaryProdRatios" sheetId="6" r:id="rId5"/>
     <sheet name="EndUseRatios" sheetId="7" r:id="rId6"/>
@@ -1270,7 +1270,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G2"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6307,7 +6307,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>